<commit_message>
Updated documentation with details on setting up Azure DevOps 7pace TimeTracker
</commit_message>
<xml_diff>
--- a/docs/Jira EXCEL.xlsx
+++ b/docs/Jira EXCEL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balazs\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!_Work\JiraWorkLogUploader\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="2019 aug" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'2019 aug'!$A$1:$E$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'2019 aug'!$A$1:$E$17</definedName>
   </definedNames>
   <calcPr calcId="162913" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
@@ -42,7 +42,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Balazs:</t>
+          <t>JIRA:</t>
         </r>
         <r>
           <rPr>
@@ -52,10 +52,35 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
--1 = TO UPLOAD
-404 = SKIP
-Filled by system (if -1 was entered):
-201 = Uploaded succesfully</t>
+-1 = SKIP, Empty = upload
+201 = Uploaded succesfully
+&gt;= 300 ERROR</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Azure DevOps 7pace:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+-1 = SKIP, Empty = upload
+200 = Uploaded succesfully
+&gt;= 300 ERROR</t>
         </r>
       </text>
     </comment>
@@ -64,14 +89,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>REFLECTION s.r.o. -&gt; PDI</t>
   </si>
   <si>
-    <t>UPS</t>
-  </si>
-  <si>
     <t>2019/8</t>
   </si>
   <si>
@@ -99,9 +121,6 @@
     <t>KS-7</t>
   </si>
   <si>
-    <t>Layout, BS, routing - Small fixes in layout CSS and one extra function: remove statically assigned opened state on mobile devices</t>
-  </si>
-  <si>
     <t>Layout, BS, routing - administrations and overhead around PR</t>
   </si>
   <si>
@@ -111,24 +130,15 @@
     <t>Packet PREH.udEmpType fix &amp; depl.</t>
   </si>
   <si>
-    <t>Packet PREH.udEmpType patch for VP &amp; depl. &amp; run (stg)</t>
-  </si>
-  <si>
     <t>PORTAL-1527</t>
   </si>
   <si>
     <t>Fix report gen. + depl.</t>
   </si>
   <si>
-    <t>Packet PREH.udEmpType fix - additional changes, conversation with James, deployment, patch</t>
-  </si>
-  <si>
     <t>OV-2</t>
   </si>
   <si>
-    <t>KS related ticket check, notes</t>
-  </si>
-  <si>
     <t>SCRUM</t>
   </si>
   <si>
@@ -138,13 +148,19 @@
     <t>PVF forms</t>
   </si>
   <si>
-    <t>PREH.udEmpType - mergees to QA, depl. - test new packet exports</t>
-  </si>
-  <si>
     <t>PREH.udEmpType - analyzing data for provided samples</t>
   </si>
   <si>
-    <t>PREH.udEmpType - changing update logic to provide list of faulty PREHs and list of PREHs not hired via HR app (avoid further chats and overhead) + furhter analisys</t>
+    <t>Jira</t>
+  </si>
+  <si>
+    <t>Azure</t>
+  </si>
+  <si>
+    <t>PREH.udEmpType - changing update logic to provide list of faulty PREHs and list of PREHs not hired via HR app (avoid further chats and overhead) + further analisys</t>
+  </si>
+  <si>
+    <t>AZURE ticket number</t>
   </si>
 </sst>
 </file>
@@ -212,12 +228,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -242,7 +264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -260,9 +282,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -278,14 +297,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -296,9 +309,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -309,9 +319,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -324,6 +331,36 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -331,7 +368,27 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -671,396 +728,370 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="102.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" style="28" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="135.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="102.33203125" style="20"/>
+    <col min="1" max="1" width="12.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="135.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="102.33203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
       <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="E2" s="11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10"/>
-      <c r="E2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="13"/>
-    </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="12"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="E4" s="12"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+    </row>
+    <row r="5" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="C5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="19"/>
-    </row>
-    <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="20"/>
-      <c r="F6" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+    </row>
+    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="16"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+    </row>
+    <row r="7" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>43678</v>
       </c>
       <c r="B7" s="3">
-        <f>SUM(B8:B15)</f>
-        <v>8.25</v>
+        <f>SUM(B8:B11)</f>
+        <v>2.75</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="E7" s="1"/>
+      <c r="F7" s="28">
+        <v>201</v>
+      </c>
+      <c r="G7" s="28">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="19"/>
+      <c r="B8" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="23">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="24"/>
-      <c r="B8" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="C8" s="25" t="s">
+      <c r="D8" s="19"/>
+      <c r="E8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="24">
+        <v>404</v>
+      </c>
+      <c r="G8" s="24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="7">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="24"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="23"/>
+      <c r="G9" s="23">
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="17">
         <v>0.5</v>
       </c>
-      <c r="C10" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="20">
+      <c r="C11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27">
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3">
-        <v>2.75</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="5" t="s">
+    <row r="12" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>43679</v>
+      </c>
+      <c r="B12" s="3">
+        <f>SUM(B13:B16)</f>
+        <v>9.5</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
+      <c r="B13" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="19"/>
+      <c r="E13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" s="3">
+        <v>2.25</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="29"/>
+      <c r="B15" s="30">
+        <v>6</v>
+      </c>
+      <c r="C15" s="31">
+        <v>873</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="33">
+        <v>-1</v>
+      </c>
+      <c r="G15" s="33"/>
+    </row>
+    <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="17">
+        <v>0</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="7">
+      <c r="D16" s="16"/>
+      <c r="E16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27">
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="23">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="19">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="19">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>43679</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="19">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="24"/>
-      <c r="B17" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="19">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="3">
-        <v>1.25</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="3">
-        <v>2.25</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="21">
-        <v>0</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="19"/>
-    </row>
-    <row r="21" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
-      <c r="F21" s="19">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
-      <c r="B22" s="1"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-    </row>
-    <row r="23" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24"/>
-      <c r="B23" s="1"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-    </row>
-    <row r="32" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="24"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-    </row>
-    <row r="33" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="24"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="24"/>
+    <row r="17" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="21"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+    </row>
+    <row r="18" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="19"/>
+      <c r="B18" s="1"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+    </row>
+    <row r="19" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="19"/>
+      <c r="B19" s="1"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+    </row>
+    <row r="28" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="19"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+    </row>
+    <row r="29" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="19"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="19"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F9 F11:F16 F19:F1048576">
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="G14:G1048576 F10:G12 F1:G8">
+    <cfRule type="cellIs" dxfId="11" priority="25" operator="greaterThanOrEqual">
       <formula>300</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="26" operator="between">
       <formula>200</formula>
       <formula>299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="27" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F17">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="G13">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThanOrEqual">
       <formula>300</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="between">
       <formula>200</formula>
       <formula>299</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18">
+  <conditionalFormatting sqref="F14:F1048576">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThanOrEqual">
+      <formula>300</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="between">
+      <formula>200</formula>
+      <formula>299</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThanOrEqual">
       <formula>300</formula>
     </cfRule>
@@ -1073,22 +1104,17 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C15" r:id="rId1" display="https://universalplant.atlassian.net/browse/OV-2"/>
-    <hyperlink ref="C8" r:id="rId2" display="https://universalplant.atlassian.net/browse/KS-7"/>
-    <hyperlink ref="C10" r:id="rId3" display="https://universalplant.atlassian.net/browse/UEPS-278"/>
-    <hyperlink ref="C11" r:id="rId4" display="https://universalplant.atlassian.net/browse/UEPS-278"/>
-    <hyperlink ref="C9" r:id="rId5" display="https://universalplant.atlassian.net/browse/KS-7"/>
-    <hyperlink ref="C12" r:id="rId6" display="https://universalplant.atlassian.net/browse/PORTAL-1527"/>
+    <hyperlink ref="C11" r:id="rId1" display="https://universalplant.atlassian.net/browse/OV-2"/>
+    <hyperlink ref="C9" r:id="rId2" display="https://universalplant.atlassian.net/browse/UEPS-278"/>
+    <hyperlink ref="C8" r:id="rId3" display="https://universalplant.atlassian.net/browse/KS-7"/>
+    <hyperlink ref="C10" r:id="rId4" display="https://universalplant.atlassian.net/browse/PORTAL-1527"/>
+    <hyperlink ref="C12" r:id="rId5" display="https://universalplant.atlassian.net/browse/UEPS-279"/>
+    <hyperlink ref="C16" r:id="rId6" display="https://universalplant.atlassian.net/browse/OV-2"/>
     <hyperlink ref="C13" r:id="rId7" display="https://universalplant.atlassian.net/browse/UEPS-278"/>
-    <hyperlink ref="C14" r:id="rId8" display="https://universalplant.atlassian.net/browse/OV-2"/>
-    <hyperlink ref="C16" r:id="rId9" display="https://universalplant.atlassian.net/browse/UEPS-279"/>
-    <hyperlink ref="C20" r:id="rId10" display="https://universalplant.atlassian.net/browse/OV-2"/>
-    <hyperlink ref="C17" r:id="rId11" display="https://universalplant.atlassian.net/browse/UEPS-278"/>
-    <hyperlink ref="C18" r:id="rId12" display="https://universalplant.atlassian.net/browse/UEPS-278"/>
-    <hyperlink ref="C19" r:id="rId13" display="https://universalplant.atlassian.net/browse/UEPS-278"/>
+    <hyperlink ref="C14" r:id="rId8" display="https://universalplant.atlassian.net/browse/UEPS-278"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="44" fitToHeight="0" orientation="portrait" r:id="rId14"/>
-  <legacyDrawing r:id="rId15"/>
+  <pageSetup paperSize="9" scale="44" fitToHeight="0" orientation="portrait" r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>